<commit_message>
test code generation module - update evaluations
</commit_message>
<xml_diff>
--- a/test-code-generator/Evaluation/QualitativeEvaluation/TemplateExperts/Baseline_UC2.4_TC1/UC2.4_TC1.evaluation.xlsx
+++ b/test-code-generator/Evaluation/QualitativeEvaluation/TemplateExperts/Baseline_UC2.4_TC1/UC2.4_TC1.evaluation.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="41">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -261,6 +261,9 @@
       </rPr>
       <t>with the correct status "passed" or "failed"</t>
     </r>
+  </si>
+  <si>
+    <t>(3) Average</t>
   </si>
   <si>
     <r>
@@ -779,9 +782,6 @@
     </r>
   </si>
   <si>
-    <t>(3) Average</t>
-  </si>
-  <si>
     <t>(2) Below average</t>
   </si>
 </sst>
@@ -4285,7 +4285,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="43.86"/>
     <col customWidth="1" min="2" max="2" width="17.0"/>
-    <col customWidth="1" min="3" max="3" width="21.29"/>
+    <col customWidth="1" min="3" max="3" width="26.43"/>
     <col customWidth="1" min="4" max="4" width="77.14"/>
     <col customWidth="1" min="5" max="26" width="8.71"/>
   </cols>
@@ -4332,7 +4332,9 @@
       <c r="A5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="8"/>
+      <c r="B5" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="C5" s="6"/>
       <c r="D5" s="10" t="s">
         <v>9</v>
@@ -4342,7 +4344,9 @@
       <c r="A6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="8"/>
+      <c r="B6" s="11" t="s">
+        <v>27</v>
+      </c>
       <c r="C6" s="8"/>
       <c r="D6" s="10" t="s">
         <v>12</v>
@@ -4352,7 +4356,9 @@
       <c r="A7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="8"/>
+      <c r="B7" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="C7" s="8"/>
       <c r="D7" s="10" t="s">
         <v>14</v>
@@ -4390,7 +4396,9 @@
       <c r="A11" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="8"/>
+      <c r="B11" s="11" t="s">
+        <v>17</v>
+      </c>
       <c r="C11" s="8"/>
       <c r="D11" s="10" t="s">
         <v>18</v>
@@ -4400,17 +4408,21 @@
       <c r="A12" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="8"/>
+      <c r="B12" s="11" t="s">
+        <v>11</v>
+      </c>
       <c r="C12" s="8"/>
       <c r="D12" s="10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="8"/>
+      <c r="B13" s="11" t="s">
+        <v>11</v>
+      </c>
       <c r="C13" s="8"/>
       <c r="D13" s="10" t="s">
         <v>22</v>
@@ -4420,20 +4432,24 @@
       <c r="A14" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="8"/>
+      <c r="B14" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="C14" s="8"/>
       <c r="D14" s="10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" ht="78.0" customHeight="1">
       <c r="A15" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
-      <c r="B15" s="8"/>
+      <c r="B15" s="11" t="s">
+        <v>11</v>
+      </c>
       <c r="C15" s="8"/>
       <c r="D15" s="10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
@@ -7472,7 +7488,9 @@
       <c r="A5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="8"/>
+      <c r="B5" s="11" t="s">
+        <v>11</v>
+      </c>
       <c r="C5" s="6"/>
       <c r="D5" s="10" t="s">
         <v>9</v>
@@ -7482,7 +7500,9 @@
       <c r="A6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="8"/>
+      <c r="B6" s="11" t="s">
+        <v>11</v>
+      </c>
       <c r="C6" s="8"/>
       <c r="D6" s="10" t="s">
         <v>12</v>
@@ -7492,7 +7512,9 @@
       <c r="A7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="8"/>
+      <c r="B7" s="11" t="s">
+        <v>11</v>
+      </c>
       <c r="C7" s="8"/>
       <c r="D7" s="10" t="s">
         <v>14</v>
@@ -7530,7 +7552,9 @@
       <c r="A11" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="8"/>
+      <c r="B11" s="11" t="s">
+        <v>17</v>
+      </c>
       <c r="C11" s="8"/>
       <c r="D11" s="10" t="s">
         <v>18</v>
@@ -7540,17 +7564,21 @@
       <c r="A12" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="8"/>
+      <c r="B12" s="11" t="s">
+        <v>11</v>
+      </c>
       <c r="C12" s="8"/>
       <c r="D12" s="10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="8"/>
+      <c r="B13" s="11" t="s">
+        <v>11</v>
+      </c>
       <c r="C13" s="8"/>
       <c r="D13" s="10" t="s">
         <v>22</v>
@@ -7563,17 +7591,19 @@
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
       <c r="D14" s="10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" ht="78.0" customHeight="1">
       <c r="A15" s="8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
-      <c r="B15" s="8"/>
+      <c r="B15" s="11" t="s">
+        <v>11</v>
+      </c>
       <c r="C15" s="8"/>
       <c r="D15" s="10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
@@ -10683,7 +10713,7 @@
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
@@ -10703,17 +10733,17 @@
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
       <c r="D14" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" ht="78.0" customHeight="1">
       <c r="A15" s="8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
       <c r="D15" s="10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
@@ -13722,7 +13752,7 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="14" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="B3" s="14"/>
     </row>

</xml_diff>